<commit_message>
chore: milestone commit for rule tuning and rewrite workflow
</commit_message>
<xml_diff>
--- a/rules_v1.xlsx
+++ b/rules_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25800" windowHeight="17655" activeTab="1"/>
+    <workbookView windowHeight="17655"/>
   </bookViews>
   <sheets>
     <sheet name="required_fields" sheetId="1" r:id="rId1"/>
@@ -384,7 +384,7 @@
     <t>施工/作业/浇筑/摊铺/开挖/吊装/张拉/压实/焊接/切割</t>
   </si>
   <si>
-    <t>项目经理/施工员/技术员/质检员/安全员/班组/监理员</t>
+    <t>项目经理/施工员/技术员/质检员/安全员/班组</t>
   </si>
   <si>
     <t>建议补充现场人员（施工单位管理人员/班组/监理人员）</t>
@@ -393,7 +393,7 @@
     <t>巡视/检查/整改/隐患/问题</t>
   </si>
   <si>
-    <t>施工单位/项目经理/安全员/班组/监理</t>
+    <t>施工单位/项目经理/安全员/班组</t>
   </si>
   <si>
     <t>低</t>
@@ -913,7 +913,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,13 +924,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1398,155 +1391,161 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1896,11 +1895,17 @@
   <sheetPr/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="73.875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -1909,7 +1914,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1932,7 +1937,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
@@ -1955,7 +1960,7 @@
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
@@ -1971,14 +1976,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" ht="67.5" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
@@ -1994,14 +1999,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" ht="135" spans="1:7">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
@@ -2028,8 +2033,8 @@
   <sheetPr/>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>

</xml_diff>